<commit_message>
Made the clusters of only top commodities and top departments according to the sales.
</commit_message>
<xml_diff>
--- a/cluster-reports/FirstIterationClusters.xlsx
+++ b/cluster-reports/FirstIterationClusters.xlsx
@@ -585,11 +585,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" zoomScale="181" zoomScaleNormal="181" zoomScalePageLayoutView="181" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="4" max="5" width="13.83203125" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="12.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B1">

</xml_diff>